<commit_message>
update presentation + create list question & answer
</commit_message>
<xml_diff>
--- a/IMS_DISK/1 - Task sheet/IMS_Tasksheet.xlsx
+++ b/IMS_DISK/1 - Task sheet/IMS_Tasksheet.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="164">
   <si>
     <t>No.</t>
   </si>
@@ -629,6 +629,12 @@
   </si>
   <si>
     <t>Report 6 - Software User's Manual</t>
+  </si>
+  <si>
+    <t>Assign location</t>
+  </si>
+  <si>
+    <t>Assign IP address range</t>
   </si>
 </sst>
 </file>
@@ -893,15 +899,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -909,10 +906,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1219,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G166"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D111" sqref="D111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1257,10 +1263,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75">
-      <c r="A2" s="35">
-        <v>1</v>
-      </c>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1274,8 +1280,8 @@
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="14" t="s">
         <v>35</v>
       </c>
@@ -1287,8 +1293,8 @@
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="15.75">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="14" t="s">
         <v>36</v>
       </c>
@@ -1300,8 +1306,8 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" ht="15.75">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="14" t="s">
         <v>19</v>
       </c>
@@ -1313,8 +1319,8 @@
       <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" ht="15.75">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="14" t="s">
         <v>37</v>
       </c>
@@ -1326,8 +1332,8 @@
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="15.75">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="14" t="s">
         <v>38</v>
       </c>
@@ -1339,8 +1345,8 @@
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" ht="15.75">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="14" t="s">
         <v>39</v>
       </c>
@@ -1352,8 +1358,8 @@
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" ht="15.75">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="14" t="s">
         <v>40</v>
       </c>
@@ -1365,10 +1371,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" ht="15.75">
-      <c r="A10" s="36">
+      <c r="A10" s="33">
         <v>2</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="33" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1382,8 +1388,8 @@
       <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" ht="15.75">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="14" t="s">
         <v>8</v>
       </c>
@@ -1395,8 +1401,8 @@
       <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" ht="15.75">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
@@ -1408,8 +1414,8 @@
       <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:7" ht="15.75">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="14" t="s">
         <v>10</v>
       </c>
@@ -1421,8 +1427,8 @@
       <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="15.75">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="14" t="s">
         <v>40</v>
       </c>
@@ -1434,10 +1440,10 @@
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="38">
+      <c r="A15" s="34">
         <v>3</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
@@ -1449,8 +1455,8 @@
       <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" ht="15.75">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="14" t="s">
         <v>41</v>
       </c>
@@ -1462,8 +1468,8 @@
       <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="15.75">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="14" t="s">
         <v>72</v>
       </c>
@@ -1475,8 +1481,8 @@
       <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="15.75">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="14" t="s">
         <v>98</v>
       </c>
@@ -1488,8 +1494,8 @@
       <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" ht="15.75">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="14" t="s">
         <v>44</v>
       </c>
@@ -1501,8 +1507,8 @@
       <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" ht="15.75">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="16" t="s">
         <v>12</v>
       </c>
@@ -1512,8 +1518,8 @@
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="15.75">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="19" t="s">
         <v>13</v>
       </c>
@@ -1525,8 +1531,8 @@
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="15.75">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="20" t="s">
         <v>45</v>
       </c>
@@ -1536,8 +1542,8 @@
       <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" ht="15.75">
-      <c r="A23" s="34"/>
-      <c r="B23" s="34"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="19" t="s">
         <v>42</v>
       </c>
@@ -1549,8 +1555,8 @@
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" ht="15.75">
-      <c r="A24" s="34"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="19" t="s">
         <v>43</v>
       </c>
@@ -1560,8 +1566,8 @@
       <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
-      <c r="A25" s="34"/>
-      <c r="B25" s="34"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="21" t="s">
         <v>99</v>
       </c>
@@ -1573,8 +1579,8 @@
       <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
-      <c r="A26" s="34"/>
-      <c r="B26" s="34"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="21" t="s">
         <v>97</v>
       </c>
@@ -1586,8 +1592,8 @@
       <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="15.75">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="21" t="s">
         <v>100</v>
       </c>
@@ -1599,8 +1605,8 @@
       <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7" ht="15.75">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="21" t="s">
         <v>101</v>
       </c>
@@ -1612,8 +1618,8 @@
       <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" ht="15.75">
-      <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="21" t="s">
         <v>102</v>
       </c>
@@ -1625,8 +1631,8 @@
       <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="15.75">
-      <c r="A30" s="34"/>
-      <c r="B30" s="34"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="21" t="s">
         <v>90</v>
       </c>
@@ -1638,8 +1644,8 @@
       <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" ht="15.75">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="21" t="s">
         <v>103</v>
       </c>
@@ -1651,8 +1657,8 @@
       <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" ht="15.75">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="21" t="s">
         <v>104</v>
       </c>
@@ -1664,8 +1670,8 @@
       <c r="G32" s="15"/>
     </row>
     <row r="33" spans="1:7" ht="15.75">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="21" t="s">
         <v>112</v>
       </c>
@@ -1677,8 +1683,8 @@
       <c r="G33" s="15"/>
     </row>
     <row r="34" spans="1:7" ht="15.75">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="21" t="s">
         <v>106</v>
       </c>
@@ -1690,8 +1696,8 @@
       <c r="G34" s="15"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="21" t="s">
         <v>108</v>
       </c>
@@ -1703,8 +1709,8 @@
       <c r="G35" s="15"/>
     </row>
     <row r="36" spans="1:7" ht="15.75">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="21" t="s">
         <v>107</v>
       </c>
@@ -1716,8 +1722,8 @@
       <c r="G36" s="15"/>
     </row>
     <row r="37" spans="1:7" ht="15.75">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="21" t="s">
         <v>105</v>
       </c>
@@ -1729,8 +1735,8 @@
       <c r="G37" s="15"/>
     </row>
     <row r="38" spans="1:7" ht="15.75">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="21" t="s">
         <v>64</v>
       </c>
@@ -1742,8 +1748,8 @@
       <c r="G38" s="15"/>
     </row>
     <row r="39" spans="1:7" ht="15.75">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="21" t="s">
         <v>109</v>
       </c>
@@ -1755,8 +1761,8 @@
       <c r="G39" s="15"/>
     </row>
     <row r="40" spans="1:7" ht="15.75">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="21" t="s">
         <v>110</v>
       </c>
@@ -1768,8 +1774,8 @@
       <c r="G40" s="15"/>
     </row>
     <row r="41" spans="1:7" ht="15.75">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="35"/>
       <c r="C41" s="21" t="s">
         <v>84</v>
       </c>
@@ -1781,8 +1787,8 @@
       <c r="G41" s="15"/>
     </row>
     <row r="42" spans="1:7" ht="15.75">
-      <c r="A42" s="34"/>
-      <c r="B42" s="34"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="21" t="s">
         <v>111</v>
       </c>
@@ -1794,8 +1800,8 @@
       <c r="G42" s="15"/>
     </row>
     <row r="43" spans="1:7" ht="15.75">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="20" t="s">
         <v>46</v>
       </c>
@@ -1807,8 +1813,8 @@
       <c r="G43" s="15"/>
     </row>
     <row r="44" spans="1:7" ht="15.75">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="19" t="s">
         <v>47</v>
       </c>
@@ -1818,8 +1824,8 @@
       <c r="G44" s="15"/>
     </row>
     <row r="45" spans="1:7" ht="15.75">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="19" t="s">
         <v>48</v>
       </c>
@@ -1829,8 +1835,8 @@
       <c r="G45" s="15"/>
     </row>
     <row r="46" spans="1:7" ht="15.75">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="19" t="s">
         <v>49</v>
       </c>
@@ -1840,8 +1846,8 @@
       <c r="G46" s="15"/>
     </row>
     <row r="47" spans="1:7" ht="15.75">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="19" t="s">
         <v>113</v>
       </c>
@@ -1853,8 +1859,8 @@
       <c r="G47" s="15"/>
     </row>
     <row r="48" spans="1:7" ht="15.75">
-      <c r="A48" s="35"/>
-      <c r="B48" s="35"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="14" t="s">
         <v>40</v>
       </c>
@@ -1866,8 +1872,8 @@
       <c r="G48" s="15"/>
     </row>
     <row r="49" spans="1:7" ht="15.75">
-      <c r="A49" s="34"/>
-      <c r="B49" s="34"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
       <c r="C49" s="14" t="s">
         <v>14</v>
       </c>
@@ -1879,8 +1885,8 @@
       <c r="G49" s="15"/>
     </row>
     <row r="50" spans="1:7" ht="15.75">
-      <c r="A50" s="34"/>
-      <c r="B50" s="34"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
       <c r="C50" s="14" t="s">
         <v>15</v>
       </c>
@@ -1892,8 +1898,8 @@
       <c r="G50" s="15"/>
     </row>
     <row r="51" spans="1:7" ht="15.75">
-      <c r="A51" s="34"/>
-      <c r="B51" s="34"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
       <c r="C51" s="16" t="s">
         <v>65</v>
       </c>
@@ -1903,8 +1909,8 @@
       <c r="G51" s="15"/>
     </row>
     <row r="52" spans="1:7" ht="15.75">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34"/>
+      <c r="A52" s="35"/>
+      <c r="B52" s="35"/>
       <c r="C52" s="30" t="s">
         <v>21</v>
       </c>
@@ -1916,8 +1922,8 @@
       <c r="G52" s="15"/>
     </row>
     <row r="53" spans="1:7" ht="15.75">
-      <c r="A53" s="34"/>
-      <c r="B53" s="34"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="35"/>
       <c r="C53" s="21" t="s">
         <v>70</v>
       </c>
@@ -1929,8 +1935,8 @@
       <c r="G53" s="15"/>
     </row>
     <row r="54" spans="1:7" ht="15.75">
-      <c r="A54" s="34"/>
-      <c r="B54" s="34"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="30" t="s">
         <v>16</v>
       </c>
@@ -1940,8 +1946,8 @@
       <c r="G54" s="15"/>
     </row>
     <row r="55" spans="1:7" ht="15.75">
-      <c r="A55" s="34"/>
-      <c r="B55" s="34"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="21" t="s">
         <v>140</v>
       </c>
@@ -1953,8 +1959,8 @@
       <c r="G55" s="15"/>
     </row>
     <row r="56" spans="1:7" ht="15.75">
-      <c r="A56" s="34"/>
-      <c r="B56" s="34"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="21" t="s">
         <v>144</v>
       </c>
@@ -1966,8 +1972,8 @@
       <c r="G56" s="15"/>
     </row>
     <row r="57" spans="1:7" ht="15.75">
-      <c r="A57" s="34"/>
-      <c r="B57" s="34"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="35"/>
       <c r="C57" s="21" t="s">
         <v>145</v>
       </c>
@@ -1979,8 +1985,8 @@
       <c r="G57" s="15"/>
     </row>
     <row r="58" spans="1:7" ht="15.75">
-      <c r="A58" s="34"/>
-      <c r="B58" s="34"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="21" t="s">
         <v>146</v>
       </c>
@@ -1992,8 +1998,8 @@
       <c r="G58" s="15"/>
     </row>
     <row r="59" spans="1:7" ht="15.75">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
       <c r="C59" s="21" t="s">
         <v>147</v>
       </c>
@@ -2005,8 +2011,8 @@
       <c r="G59" s="15"/>
     </row>
     <row r="60" spans="1:7" ht="15.75">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="35"/>
       <c r="C60" s="21" t="s">
         <v>148</v>
       </c>
@@ -2018,8 +2024,8 @@
       <c r="G60" s="15"/>
     </row>
     <row r="61" spans="1:7" ht="15.75">
-      <c r="A61" s="34"/>
-      <c r="B61" s="34"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="35"/>
       <c r="C61" s="21" t="s">
         <v>149</v>
       </c>
@@ -2031,8 +2037,8 @@
       <c r="G61" s="15"/>
     </row>
     <row r="62" spans="1:7" ht="15.75">
-      <c r="A62" s="34"/>
-      <c r="B62" s="34"/>
+      <c r="A62" s="35"/>
+      <c r="B62" s="35"/>
       <c r="C62" s="21" t="s">
         <v>150</v>
       </c>
@@ -2044,8 +2050,8 @@
       <c r="G62" s="15"/>
     </row>
     <row r="63" spans="1:7" ht="15.75">
-      <c r="A63" s="34"/>
-      <c r="B63" s="34"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="35"/>
       <c r="C63" s="21" t="s">
         <v>151</v>
       </c>
@@ -2057,8 +2063,8 @@
       <c r="G63" s="15"/>
     </row>
     <row r="64" spans="1:7" ht="15.75">
-      <c r="A64" s="34"/>
-      <c r="B64" s="34"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="35"/>
       <c r="C64" s="21" t="s">
         <v>143</v>
       </c>
@@ -2070,8 +2076,8 @@
       <c r="G64" s="15"/>
     </row>
     <row r="65" spans="1:7" ht="15.75">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="35"/>
       <c r="C65" s="21" t="s">
         <v>152</v>
       </c>
@@ -2083,8 +2089,8 @@
       <c r="G65" s="15"/>
     </row>
     <row r="66" spans="1:7" ht="15.75">
-      <c r="A66" s="34"/>
-      <c r="B66" s="34"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="35"/>
       <c r="C66" s="21" t="s">
         <v>153</v>
       </c>
@@ -2096,8 +2102,8 @@
       <c r="G66" s="15"/>
     </row>
     <row r="67" spans="1:7" ht="15.75">
-      <c r="A67" s="34"/>
-      <c r="B67" s="34"/>
+      <c r="A67" s="35"/>
+      <c r="B67" s="35"/>
       <c r="C67" s="21" t="s">
         <v>154</v>
       </c>
@@ -2109,8 +2115,8 @@
       <c r="G67" s="15"/>
     </row>
     <row r="68" spans="1:7" ht="15.75">
-      <c r="A68" s="34"/>
-      <c r="B68" s="34"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="35"/>
       <c r="C68" s="21" t="s">
         <v>155</v>
       </c>
@@ -2122,8 +2128,8 @@
       <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:7" ht="15.75">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="35"/>
       <c r="C69" s="21" t="s">
         <v>156</v>
       </c>
@@ -2135,8 +2141,8 @@
       <c r="G69" s="15"/>
     </row>
     <row r="70" spans="1:7" ht="15.75">
-      <c r="A70" s="34"/>
-      <c r="B70" s="34"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="35"/>
       <c r="C70" s="21" t="s">
         <v>157</v>
       </c>
@@ -2148,8 +2154,8 @@
       <c r="G70" s="15"/>
     </row>
     <row r="71" spans="1:7" ht="15.75">
-      <c r="A71" s="34"/>
-      <c r="B71" s="34"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="35"/>
       <c r="C71" s="21" t="s">
         <v>142</v>
       </c>
@@ -2161,8 +2167,8 @@
       <c r="G71" s="15"/>
     </row>
     <row r="72" spans="1:7" ht="15.75">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
+      <c r="A72" s="35"/>
+      <c r="B72" s="35"/>
       <c r="C72" s="21" t="s">
         <v>160</v>
       </c>
@@ -2174,8 +2180,8 @@
       <c r="G72" s="15"/>
     </row>
     <row r="73" spans="1:7" ht="15.75">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="21" t="s">
         <v>141</v>
       </c>
@@ -2187,8 +2193,8 @@
       <c r="G73" s="15"/>
     </row>
     <row r="74" spans="1:7" ht="15.75">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
+      <c r="A74" s="35"/>
+      <c r="B74" s="35"/>
       <c r="C74" s="21" t="s">
         <v>158</v>
       </c>
@@ -2200,8 +2206,8 @@
       <c r="G74" s="15"/>
     </row>
     <row r="75" spans="1:7" ht="15.75">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
+      <c r="A75" s="35"/>
+      <c r="B75" s="35"/>
       <c r="C75" s="21" t="s">
         <v>159</v>
       </c>
@@ -2213,8 +2219,8 @@
       <c r="G75" s="15"/>
     </row>
     <row r="76" spans="1:7" ht="15.75">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="35"/>
       <c r="C76" s="31" t="s">
         <v>66</v>
       </c>
@@ -2224,8 +2230,8 @@
       <c r="G76" s="15"/>
     </row>
     <row r="77" spans="1:7" ht="15.75">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
+      <c r="A77" s="35"/>
+      <c r="B77" s="35"/>
       <c r="C77" s="16" t="s">
         <v>67</v>
       </c>
@@ -2235,8 +2241,8 @@
       <c r="G77" s="15"/>
     </row>
     <row r="78" spans="1:7" ht="15.75">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
+      <c r="A78" s="35"/>
+      <c r="B78" s="35"/>
       <c r="C78" s="17" t="s">
         <v>68</v>
       </c>
@@ -2248,8 +2254,8 @@
       <c r="G78" s="15"/>
     </row>
     <row r="79" spans="1:7" ht="15.75">
-      <c r="A79" s="34"/>
-      <c r="B79" s="34"/>
+      <c r="A79" s="35"/>
+      <c r="B79" s="35"/>
       <c r="C79" s="17" t="s">
         <v>69</v>
       </c>
@@ -2261,8 +2267,8 @@
       <c r="G79" s="15"/>
     </row>
     <row r="80" spans="1:7" ht="15.75">
-      <c r="A80" s="34"/>
-      <c r="B80" s="34"/>
+      <c r="A80" s="35"/>
+      <c r="B80" s="35"/>
       <c r="C80" s="31" t="s">
         <v>20</v>
       </c>
@@ -2272,8 +2278,8 @@
       <c r="G80" s="15"/>
     </row>
     <row r="81" spans="1:7" ht="15.75">
-      <c r="A81" s="34"/>
-      <c r="B81" s="34"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
       <c r="C81" s="17" t="s">
         <v>114</v>
       </c>
@@ -2285,8 +2291,8 @@
       <c r="G81" s="15"/>
     </row>
     <row r="82" spans="1:7" ht="15.75">
-      <c r="A82" s="34"/>
-      <c r="B82" s="34"/>
+      <c r="A82" s="35"/>
+      <c r="B82" s="35"/>
       <c r="C82" s="17" t="s">
         <v>115</v>
       </c>
@@ -2298,8 +2304,8 @@
       <c r="G82" s="15"/>
     </row>
     <row r="83" spans="1:7" ht="15.75">
-      <c r="A83" s="34"/>
-      <c r="B83" s="34"/>
+      <c r="A83" s="35"/>
+      <c r="B83" s="35"/>
       <c r="C83" s="17" t="s">
         <v>116</v>
       </c>
@@ -2311,8 +2317,8 @@
       <c r="G83" s="15"/>
     </row>
     <row r="84" spans="1:7" ht="15.75">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
+      <c r="A84" s="35"/>
+      <c r="B84" s="35"/>
       <c r="C84" s="17" t="s">
         <v>117</v>
       </c>
@@ -2324,8 +2330,8 @@
       <c r="G84" s="15"/>
     </row>
     <row r="85" spans="1:7" ht="15.75">
-      <c r="A85" s="34"/>
-      <c r="B85" s="34"/>
+      <c r="A85" s="35"/>
+      <c r="B85" s="35"/>
       <c r="C85" s="17" t="s">
         <v>118</v>
       </c>
@@ -2337,8 +2343,8 @@
       <c r="G85" s="15"/>
     </row>
     <row r="86" spans="1:7" ht="15.75">
-      <c r="A86" s="34"/>
-      <c r="B86" s="34"/>
+      <c r="A86" s="35"/>
+      <c r="B86" s="35"/>
       <c r="C86" s="17" t="s">
         <v>119</v>
       </c>
@@ -2350,8 +2356,8 @@
       <c r="G86" s="15"/>
     </row>
     <row r="87" spans="1:7" ht="15.75">
-      <c r="A87" s="34"/>
-      <c r="B87" s="34"/>
+      <c r="A87" s="35"/>
+      <c r="B87" s="35"/>
       <c r="C87" s="17" t="s">
         <v>120</v>
       </c>
@@ -2363,8 +2369,8 @@
       <c r="G87" s="15"/>
     </row>
     <row r="88" spans="1:7" ht="15.75">
-      <c r="A88" s="35"/>
-      <c r="B88" s="35"/>
+      <c r="A88" s="32"/>
+      <c r="B88" s="32"/>
       <c r="C88" s="14" t="s">
         <v>40</v>
       </c>
@@ -2376,10 +2382,10 @@
       <c r="G88" s="15"/>
     </row>
     <row r="89" spans="1:7" ht="15.75">
-      <c r="A89" s="37">
+      <c r="A89" s="36">
         <v>5</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="33" t="s">
         <v>22</v>
       </c>
       <c r="C89" s="16" t="s">
@@ -2391,8 +2397,8 @@
       <c r="G89" s="15"/>
     </row>
     <row r="90" spans="1:7" ht="15.75">
-      <c r="A90" s="32"/>
-      <c r="B90" s="36"/>
+      <c r="A90" s="38"/>
+      <c r="B90" s="33"/>
       <c r="C90" s="17" t="s">
         <v>74</v>
       </c>
@@ -2404,8 +2410,8 @@
       <c r="G90" s="15"/>
     </row>
     <row r="91" spans="1:7" ht="15.75">
-      <c r="A91" s="32"/>
-      <c r="B91" s="36"/>
+      <c r="A91" s="38"/>
+      <c r="B91" s="33"/>
       <c r="C91" s="17" t="s">
         <v>69</v>
       </c>
@@ -2417,8 +2423,8 @@
       <c r="G91" s="15"/>
     </row>
     <row r="92" spans="1:7" ht="15.75">
-      <c r="A92" s="32"/>
-      <c r="B92" s="36"/>
+      <c r="A92" s="38"/>
+      <c r="B92" s="33"/>
       <c r="C92" s="16" t="s">
         <v>95</v>
       </c>
@@ -2434,8 +2440,8 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="15.75">
-      <c r="A93" s="32"/>
-      <c r="B93" s="36"/>
+      <c r="A93" s="38"/>
+      <c r="B93" s="33"/>
       <c r="C93" s="16" t="s">
         <v>75</v>
       </c>
@@ -2445,8 +2451,8 @@
       <c r="G93" s="15"/>
     </row>
     <row r="94" spans="1:7" ht="15.75">
-      <c r="A94" s="32"/>
-      <c r="B94" s="36"/>
+      <c r="A94" s="38"/>
+      <c r="B94" s="33"/>
       <c r="C94" s="17" t="s">
         <v>97</v>
       </c>
@@ -2462,8 +2468,8 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="15.75">
-      <c r="A95" s="32"/>
-      <c r="B95" s="36"/>
+      <c r="A95" s="38"/>
+      <c r="B95" s="33"/>
       <c r="C95" s="17" t="s">
         <v>90</v>
       </c>
@@ -2479,8 +2485,8 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="15.75">
-      <c r="A96" s="32"/>
-      <c r="B96" s="36"/>
+      <c r="A96" s="38"/>
+      <c r="B96" s="33"/>
       <c r="C96" s="17" t="s">
         <v>103</v>
       </c>
@@ -2496,8 +2502,8 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="15.75">
-      <c r="A97" s="32"/>
-      <c r="B97" s="36"/>
+      <c r="A97" s="38"/>
+      <c r="B97" s="33"/>
       <c r="C97" s="17" t="s">
         <v>92</v>
       </c>
@@ -2513,8 +2519,8 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="15.75">
-      <c r="A98" s="32"/>
-      <c r="B98" s="36"/>
+      <c r="A98" s="38"/>
+      <c r="B98" s="33"/>
       <c r="C98" s="16" t="s">
         <v>124</v>
       </c>
@@ -2524,8 +2530,8 @@
       <c r="G98" s="15"/>
     </row>
     <row r="99" spans="1:7" ht="15.75">
-      <c r="A99" s="32"/>
-      <c r="B99" s="36"/>
+      <c r="A99" s="38"/>
+      <c r="B99" s="33"/>
       <c r="C99" s="17" t="s">
         <v>125</v>
       </c>
@@ -2541,8 +2547,8 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="15.75">
-      <c r="A100" s="32"/>
-      <c r="B100" s="36"/>
+      <c r="A100" s="38"/>
+      <c r="B100" s="33"/>
       <c r="C100" s="17" t="s">
         <v>126</v>
       </c>
@@ -2558,8 +2564,8 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="15.75">
-      <c r="A101" s="32"/>
-      <c r="B101" s="36"/>
+      <c r="A101" s="38"/>
+      <c r="B101" s="33"/>
       <c r="C101" s="17" t="s">
         <v>127</v>
       </c>
@@ -2575,8 +2581,8 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="15.75">
-      <c r="A102" s="32"/>
-      <c r="B102" s="36"/>
+      <c r="A102" s="38"/>
+      <c r="B102" s="33"/>
       <c r="C102" s="16" t="s">
         <v>128</v>
       </c>
@@ -2586,8 +2592,8 @@
       <c r="G102" s="15"/>
     </row>
     <row r="103" spans="1:7" ht="15.75">
-      <c r="A103" s="32"/>
-      <c r="B103" s="36"/>
+      <c r="A103" s="38"/>
+      <c r="B103" s="33"/>
       <c r="C103" s="17" t="s">
         <v>93</v>
       </c>
@@ -2603,8 +2609,8 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.75">
-      <c r="A104" s="32"/>
-      <c r="B104" s="36"/>
+      <c r="A104" s="38"/>
+      <c r="B104" s="33"/>
       <c r="C104" s="17" t="s">
         <v>129</v>
       </c>
@@ -2620,8 +2626,8 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="15.75">
-      <c r="A105" s="32"/>
-      <c r="B105" s="36"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="33"/>
       <c r="C105" s="17" t="s">
         <v>131</v>
       </c>
@@ -2637,8 +2643,8 @@
       </c>
     </row>
     <row r="106" spans="1:7" ht="15.75">
-      <c r="A106" s="32"/>
-      <c r="B106" s="36"/>
+      <c r="A106" s="38"/>
+      <c r="B106" s="33"/>
       <c r="C106" s="17" t="s">
         <v>121</v>
       </c>
@@ -2654,8 +2660,8 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15.75">
-      <c r="A107" s="32"/>
-      <c r="B107" s="36"/>
+      <c r="A107" s="38"/>
+      <c r="B107" s="33"/>
       <c r="C107" s="17" t="s">
         <v>102</v>
       </c>
@@ -2671,8 +2677,8 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75">
-      <c r="A108" s="32"/>
-      <c r="B108" s="36"/>
+      <c r="A108" s="38"/>
+      <c r="B108" s="33"/>
       <c r="C108" s="17" t="s">
         <v>135</v>
       </c>
@@ -2688,8 +2694,8 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="15.75">
-      <c r="A109" s="32"/>
-      <c r="B109" s="36"/>
+      <c r="A109" s="38"/>
+      <c r="B109" s="33"/>
       <c r="C109" s="17" t="s">
         <v>136</v>
       </c>
@@ -2705,8 +2711,8 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="15.75">
-      <c r="A110" s="32"/>
-      <c r="B110" s="36"/>
+      <c r="A110" s="38"/>
+      <c r="B110" s="33"/>
       <c r="C110" s="17" t="s">
         <v>130</v>
       </c>
@@ -2722,8 +2728,8 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.75">
-      <c r="A111" s="32"/>
-      <c r="B111" s="36"/>
+      <c r="A111" s="38"/>
+      <c r="B111" s="33"/>
       <c r="C111" s="17" t="s">
         <v>137</v>
       </c>
@@ -2739,8 +2745,8 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="15.75">
-      <c r="A112" s="32"/>
-      <c r="B112" s="36"/>
+      <c r="A112" s="38"/>
+      <c r="B112" s="33"/>
       <c r="C112" s="17" t="s">
         <v>105</v>
       </c>
@@ -2756,10 +2762,10 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.75">
-      <c r="A113" s="32"/>
-      <c r="B113" s="36"/>
+      <c r="A113" s="38"/>
+      <c r="B113" s="33"/>
       <c r="C113" s="17" t="s">
-        <v>110</v>
+        <v>162</v>
       </c>
       <c r="D113" s="12"/>
       <c r="E113" s="12" t="s">
@@ -2773,10 +2779,10 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="15.75">
-      <c r="A114" s="32"/>
-      <c r="B114" s="36"/>
+      <c r="A114" s="38"/>
+      <c r="B114" s="33"/>
       <c r="C114" s="17" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D114" s="12"/>
       <c r="E114" s="12" t="s">
@@ -2786,14 +2792,14 @@
         <v>1</v>
       </c>
       <c r="G114" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.75">
-      <c r="A115" s="32"/>
-      <c r="B115" s="36"/>
+      <c r="A115" s="38"/>
+      <c r="B115" s="33"/>
       <c r="C115" s="17" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="D115" s="12"/>
       <c r="E115" s="12" t="s">
@@ -2803,14 +2809,14 @@
         <v>1</v>
       </c>
       <c r="G115" s="15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15.75">
-      <c r="A116" s="32"/>
-      <c r="B116" s="36"/>
+      <c r="A116" s="38"/>
+      <c r="B116" s="33"/>
       <c r="C116" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D116" s="12"/>
       <c r="E116" s="12" t="s">
@@ -2820,31 +2826,31 @@
         <v>1</v>
       </c>
       <c r="G116" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.75">
-      <c r="A117" s="32"/>
-      <c r="B117" s="36"/>
+      <c r="A117" s="38"/>
+      <c r="B117" s="33"/>
       <c r="C117" s="17" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="D117" s="12"/>
       <c r="E117" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F117" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G117" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.75">
-      <c r="A118" s="32"/>
-      <c r="B118" s="36"/>
+      <c r="A118" s="38"/>
+      <c r="B118" s="33"/>
       <c r="C118" s="17" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D118" s="12"/>
       <c r="E118" s="12" t="s">
@@ -2854,104 +2860,104 @@
         <v>1</v>
       </c>
       <c r="G118" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="15.75">
+      <c r="A119" s="38"/>
+      <c r="B119" s="33"/>
+      <c r="C119" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F119" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" ht="15.75">
-      <c r="A119" s="32"/>
-      <c r="B119" s="36"/>
-      <c r="C119" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="15"/>
-      <c r="G119" s="15"/>
+      <c r="G119" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" spans="1:7" ht="15.75">
-      <c r="A120" s="32"/>
-      <c r="B120" s="36"/>
+      <c r="A120" s="38"/>
+      <c r="B120" s="33"/>
       <c r="C120" s="17" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D120" s="12"/>
       <c r="E120" s="12" t="s">
         <v>6</v>
       </c>
       <c r="F120" s="15">
+        <v>1</v>
+      </c>
+      <c r="G120" s="15">
         <v>2</v>
       </c>
-      <c r="G120" s="15">
+    </row>
+    <row r="121" spans="1:7" ht="15.75">
+      <c r="A121" s="38"/>
+      <c r="B121" s="33"/>
+      <c r="C121" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+    </row>
+    <row r="122" spans="1:7" ht="15.75">
+      <c r="A122" s="38"/>
+      <c r="B122" s="33"/>
+      <c r="C122" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F122" s="15">
+        <v>2</v>
+      </c>
+      <c r="G122" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15.75">
-      <c r="A121" s="32"/>
-      <c r="B121" s="36"/>
-      <c r="C121" s="17" t="s">
+    <row r="123" spans="1:7" ht="15.75">
+      <c r="A123" s="38"/>
+      <c r="B123" s="33"/>
+      <c r="C123" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D121" s="12"/>
-      <c r="E121" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F121" s="15">
-        <v>1</v>
-      </c>
-      <c r="G121" s="15">
+      <c r="D123" s="12"/>
+      <c r="E123" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F123" s="15">
+        <v>1</v>
+      </c>
+      <c r="G123" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15.75">
-      <c r="A122" s="32"/>
-      <c r="B122" s="36"/>
-      <c r="C122" s="16" t="s">
+    <row r="124" spans="1:7" ht="15.75">
+      <c r="A124" s="38"/>
+      <c r="B124" s="33"/>
+      <c r="C124" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D122" s="12"/>
-      <c r="E122" s="12"/>
-      <c r="F122" s="15"/>
-      <c r="G122" s="15"/>
-    </row>
-    <row r="123" spans="1:7" ht="15.75">
-      <c r="A123" s="32"/>
-      <c r="B123" s="36"/>
-      <c r="C123" s="17" t="s">
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+    </row>
+    <row r="125" spans="1:7" ht="15.75">
+      <c r="A125" s="38"/>
+      <c r="B125" s="33"/>
+      <c r="C125" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E123" s="12"/>
-      <c r="F123" s="15">
-        <v>7</v>
-      </c>
-      <c r="G123" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="15.75">
-      <c r="A124" s="32"/>
-      <c r="B124" s="36"/>
-      <c r="C124" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D124" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E124" s="12"/>
-      <c r="F124" s="15">
-        <v>7</v>
-      </c>
-      <c r="G124" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="15.75">
-      <c r="A125" s="32"/>
-      <c r="B125" s="36"/>
-      <c r="C125" s="17" t="s">
-        <v>138</v>
       </c>
       <c r="D125" s="12" t="s">
         <v>6</v>
@@ -2961,53 +2967,53 @@
         <v>7</v>
       </c>
       <c r="G125" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15.75">
-      <c r="A126" s="32"/>
-      <c r="B126" s="36"/>
+      <c r="A126" s="38"/>
+      <c r="B126" s="33"/>
       <c r="C126" s="17" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D126" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E126" s="12"/>
       <c r="F126" s="15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G126" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15.75">
-      <c r="A127" s="32"/>
-      <c r="B127" s="36"/>
+      <c r="A127" s="38"/>
+      <c r="B127" s="33"/>
       <c r="C127" s="17" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D127" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E127" s="12"/>
       <c r="F127" s="15">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G127" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15.75">
-      <c r="A128" s="32"/>
-      <c r="B128" s="36"/>
+      <c r="A128" s="38"/>
+      <c r="B128" s="33"/>
       <c r="C128" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D128" s="12"/>
-      <c r="E128" s="12" t="s">
-        <v>6</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" s="12"/>
       <c r="F128" s="15">
         <v>1</v>
       </c>
@@ -3016,21 +3022,27 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="15.75">
-      <c r="A129" s="32"/>
-      <c r="B129" s="36"/>
-      <c r="C129" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D129" s="12"/>
+      <c r="A129" s="38"/>
+      <c r="B129" s="33"/>
+      <c r="C129" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="E129" s="12"/>
-      <c r="F129" s="15"/>
-      <c r="G129" s="15"/>
+      <c r="F129" s="15">
+        <v>1</v>
+      </c>
+      <c r="G129" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="130" spans="1:7" ht="15.75">
-      <c r="A130" s="32"/>
-      <c r="B130" s="36"/>
+      <c r="A130" s="38"/>
+      <c r="B130" s="33"/>
       <c r="C130" s="17" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D130" s="12"/>
       <c r="E130" s="12" t="s">
@@ -3040,31 +3052,25 @@
         <v>1</v>
       </c>
       <c r="G130" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.75">
-      <c r="A131" s="32"/>
-      <c r="B131" s="36"/>
-      <c r="C131" s="17" t="s">
-        <v>83</v>
+      <c r="A131" s="38"/>
+      <c r="B131" s="33"/>
+      <c r="C131" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="D131" s="12"/>
-      <c r="E131" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F131" s="15">
-        <v>1</v>
-      </c>
-      <c r="G131" s="15">
-        <v>1</v>
-      </c>
+      <c r="E131" s="12"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
     </row>
     <row r="132" spans="1:7" ht="15.75">
-      <c r="A132" s="32"/>
-      <c r="B132" s="36"/>
+      <c r="A132" s="38"/>
+      <c r="B132" s="33"/>
       <c r="C132" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D132" s="12"/>
       <c r="E132" s="12" t="s">
@@ -3078,10 +3084,10 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="15.75">
-      <c r="A133" s="32"/>
-      <c r="B133" s="36"/>
+      <c r="A133" s="38"/>
+      <c r="B133" s="33"/>
       <c r="C133" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D133" s="12"/>
       <c r="E133" s="12" t="s">
@@ -3095,10 +3101,10 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="15.75">
-      <c r="A134" s="32"/>
-      <c r="B134" s="36"/>
+      <c r="A134" s="38"/>
+      <c r="B134" s="33"/>
       <c r="C134" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D134" s="12"/>
       <c r="E134" s="12" t="s">
@@ -3108,209 +3114,215 @@
         <v>1</v>
       </c>
       <c r="G134" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="15.75">
-      <c r="A135" s="32"/>
-      <c r="B135" s="36"/>
-      <c r="C135" s="16" t="s">
-        <v>132</v>
+      <c r="A135" s="38"/>
+      <c r="B135" s="33"/>
+      <c r="C135" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="D135" s="12"/>
-      <c r="E135" s="12"/>
-      <c r="F135" s="15"/>
-      <c r="G135" s="15"/>
+      <c r="E135" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F135" s="15">
+        <v>1</v>
+      </c>
+      <c r="G135" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" spans="1:7" ht="15.75">
-      <c r="A136" s="32"/>
-      <c r="B136" s="36"/>
+      <c r="A136" s="38"/>
+      <c r="B136" s="33"/>
       <c r="C136" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D136" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E136" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="D136" s="12"/>
+      <c r="E136" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="F136" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G136" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="15.75">
-      <c r="A137" s="32"/>
-      <c r="B137" s="36"/>
-      <c r="C137" s="17" t="s">
+      <c r="A137" s="38"/>
+      <c r="B137" s="33"/>
+      <c r="C137" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D137" s="12"/>
+      <c r="E137" s="12"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="15"/>
+    </row>
+    <row r="138" spans="1:7" ht="15.75">
+      <c r="A138" s="38"/>
+      <c r="B138" s="33"/>
+      <c r="C138" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D138" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" s="12"/>
+      <c r="F138" s="15">
+        <v>3</v>
+      </c>
+      <c r="G138" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="15.75">
+      <c r="A139" s="38"/>
+      <c r="B139" s="33"/>
+      <c r="C139" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="D137" s="12"/>
-      <c r="E137" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F137" s="15">
-        <v>1</v>
-      </c>
-      <c r="G137" s="15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="15.75">
-      <c r="A138" s="32"/>
-      <c r="B138" s="36"/>
-      <c r="C138" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D138" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E138" s="12"/>
-      <c r="F138" s="15"/>
-      <c r="G138" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="15.75">
-      <c r="A139" s="32"/>
-      <c r="B139" s="36"/>
-      <c r="C139" s="31" t="s">
-        <v>94</v>
       </c>
       <c r="D139" s="12"/>
       <c r="E139" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F139" s="15"/>
+      <c r="F139" s="15">
+        <v>1</v>
+      </c>
       <c r="G139" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="15.75">
+      <c r="A140" s="38"/>
+      <c r="B140" s="33"/>
+      <c r="C140" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" s="12"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="15.75">
+      <c r="A141" s="38"/>
+      <c r="B141" s="33"/>
+      <c r="C141" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D141" s="12"/>
+      <c r="E141" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F141" s="15"/>
+      <c r="G141" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15.75">
-      <c r="A140" s="32"/>
-      <c r="B140" s="36"/>
-      <c r="C140" s="31" t="s">
+    <row r="142" spans="1:7" ht="15.75">
+      <c r="A142" s="38"/>
+      <c r="B142" s="33"/>
+      <c r="C142" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D140" s="12"/>
-      <c r="E140" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F140" s="15"/>
-      <c r="G140" s="15"/>
-    </row>
-    <row r="141" spans="1:7" ht="15.75">
-      <c r="A141" s="32"/>
-      <c r="B141" s="36"/>
-      <c r="C141" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="D141" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E141" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F141" s="15"/>
-      <c r="G141" s="15"/>
-    </row>
-    <row r="142" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A142" s="37">
-        <v>6</v>
-      </c>
-      <c r="B142" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C142" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D142" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E142" s="12"/>
+      <c r="D142" s="12"/>
+      <c r="E142" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="F142" s="15"/>
       <c r="G142" s="15"/>
     </row>
     <row r="143" spans="1:7" ht="15.75">
-      <c r="A143" s="33"/>
-      <c r="B143" s="36"/>
-      <c r="C143" s="18" t="s">
-        <v>80</v>
+      <c r="A143" s="38"/>
+      <c r="B143" s="33"/>
+      <c r="C143" s="31" t="s">
+        <v>18</v>
       </c>
       <c r="D143" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E143" s="12"/>
+      <c r="E143" s="12" t="s">
+        <v>6</v>
+      </c>
       <c r="F143" s="15"/>
       <c r="G143" s="15"/>
     </row>
-    <row r="144" spans="1:7">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="18"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="G144" s="2"/>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B145" s="2"/>
-      <c r="C145" s="1"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="G145" s="2"/>
+    <row r="144" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A144" s="36">
+        <v>6</v>
+      </c>
+      <c r="B144" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" s="12"/>
+      <c r="F144" s="15"/>
+      <c r="G144" s="15"/>
+    </row>
+    <row r="145" spans="1:7" ht="15.75">
+      <c r="A145" s="37"/>
+      <c r="B145" s="33"/>
+      <c r="C145" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="12"/>
+      <c r="F145" s="15"/>
+      <c r="G145" s="15"/>
     </row>
     <row r="146" spans="1:7">
-      <c r="A146" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C146" s="1"/>
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="18"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
       <c r="G146" s="2"/>
     </row>
-    <row r="147" spans="1:7" ht="60">
-      <c r="A147" s="5">
-        <v>1</v>
-      </c>
-      <c r="B147" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>27</v>
-      </c>
+    <row r="147" spans="1:7">
+      <c r="A147" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" s="1"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
       <c r="G147" s="2"/>
     </row>
-    <row r="148" spans="1:7" ht="30">
-      <c r="A148" s="7">
-        <v>2</v>
-      </c>
-      <c r="B148" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C148" s="3">
-        <v>1</v>
-      </c>
+    <row r="148" spans="1:7">
+      <c r="A148" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148" s="1"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
       <c r="G148" s="2"/>
     </row>
-    <row r="149" spans="1:7" ht="30">
-      <c r="A149" s="7">
-        <v>3</v>
+    <row r="149" spans="1:7" ht="60">
+      <c r="A149" s="5">
+        <v>1</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C149" s="7">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -3318,13 +3330,13 @@
     </row>
     <row r="150" spans="1:7" ht="30">
       <c r="A150" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C150" s="7">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="C150" s="3">
+        <v>1</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -3332,32 +3344,50 @@
     </row>
     <row r="151" spans="1:7" ht="30">
       <c r="A151" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C151" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
       <c r="G151" s="2"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" ht="30">
+      <c r="A152" s="7">
+        <v>4</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C152" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
       <c r="G152" s="2"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" ht="30">
+      <c r="A153" s="7">
+        <v>5</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C153" s="7">
+        <v>4</v>
+      </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
       <c r="G153" s="2"/>
     </row>
     <row r="154" spans="1:7">
+      <c r="C154" s="7">
+        <v>5</v>
+      </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="G154" s="2"/>
@@ -3422,23 +3452,33 @@
       <c r="E166" s="2"/>
       <c r="G166" s="2"/>
     </row>
+    <row r="167" spans="4:7">
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="G167" s="2"/>
+    </row>
+    <row r="168" spans="4:7">
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="G168" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="B89:B143"/>
+    <mergeCell ref="A89:A143"/>
+    <mergeCell ref="B49:B88"/>
+    <mergeCell ref="A49:A88"/>
     <mergeCell ref="B2:B9"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A48"/>
     <mergeCell ref="B15:B48"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="B89:B141"/>
-    <mergeCell ref="A89:A141"/>
-    <mergeCell ref="B49:B88"/>
-    <mergeCell ref="A49:A88"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E164">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E166">
       <formula1>"O, "</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>